<commit_message>
update CIL (SIQ v1.2)
</commit_message>
<xml_diff>
--- a/2-Reqs/ConfigurationItemList.xlsx
+++ b/2-Reqs/ConfigurationItemList.xlsx
@@ -200,7 +200,7 @@
     <t>https://github.com/sohip-a/Foodies/blob/main/2-Reqs/SIQ/SIQ22-02-2023.xlsx</t>
   </si>
   <si>
-    <t>V 1.1</t>
+    <t>V 1.2</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update RTM in CIL
</commit_message>
<xml_diff>
--- a/2-Reqs/ConfigurationItemList.xlsx
+++ b/2-Reqs/ConfigurationItemList.xlsx
@@ -178,9 +178,6 @@
     <t>RTM.xlsx</t>
   </si>
   <si>
-    <t>https://github.com/sohip-a/Foodies/blob/main/1-%20PM/RTM.xlsx</t>
-  </si>
-  <si>
     <t>SIQ18-02-2023.xlsx</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>V 1.2</t>
+  </si>
+  <si>
+    <t>https://github.com/sohip-a/Foodies/blob/main/2-Reqs/RTM.xlsx</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -839,10 +839,10 @@
         <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>19</v>
@@ -854,7 +854,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>15</v>
@@ -1164,7 +1164,7 @@
         <v>52</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>47</v>
@@ -1176,7 +1176,7 @@
         <v>14</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>15</v>
@@ -1204,13 +1204,13 @@
     </row>
     <row r="13" spans="1:26" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="C13" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>19</v>
@@ -1219,10 +1219,10 @@
         <v>13</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>15</v>

</xml_diff>